<commit_message>
- catálogo productos, crud, exportar(excel, pdf), filtros, detalles, etc
Signed-off-by: softcode-seo <miguellopez@softcode.com.mx>
</commit_message>
<xml_diff>
--- a/public/assets/plantillas/plantilla_categorias.xlsx
+++ b/public/assets/plantillas/plantilla_categorias.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROYECTOS\myBusinessFaster\public\assets\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517E9FDB-AEBB-49D3-A47C-1B0C2ED4917B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3824CDC0-F138-41FE-8677-7DDD0E01C9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11520" xr2:uid="{34376D26-84E7-4B9C-AE2C-1B71B7AC8B83}"/>
   </bookViews>
@@ -74,9 +74,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -88,13 +86,28 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -105,6 +118,16 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9C4B354D-FB92-4D16-AEFE-63239FAB6383}" name="Tabla2" displayName="Tabla2" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowBorderDxfId="0" tableBorderDxfId="1">
+  <autoFilter ref="A1:A2" xr:uid="{9C4B354D-FB92-4D16-AEFE-63239FAB6383}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{BA918BAC-E728-48EB-BF1A-D6E0505021F3}" name="categoria"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -407,7 +430,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,12 +439,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>